<commit_message>
BF: ignore xlsx files
</commit_message>
<xml_diff>
--- a/Resolution_matrix_summary.xlsx
+++ b/Resolution_matrix_summary.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexhe/Desktop/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexhe/Dropbox (Personal)/Active_projects/Asilomar_srcloc/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3738C90-AE80-4149-9EED-CF23338DA84E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7BFE993A-2A68-8E4A-92C1-DA9AEFED6845}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="34400" yWindow="500" windowWidth="34400" windowHeight="26400" xr2:uid="{ED3615AD-61CD-584C-9FC1-61A5A4F071FE}"/>
   </bookViews>
@@ -548,7 +548,7 @@
   <dimension ref="A1:I17"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="172" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="D23" sqref="D23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>